<commit_message>
added Feb 6 2024 results
</commit_message>
<xml_diff>
--- a/screener.xlsx
+++ b/screener.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\stocks\pse-edge-parser\pse-edge-parser\"/>
     </mc:Choice>
@@ -21,13 +21,14 @@
     <sheet name="05Oct2021 223307" sheetId="6" r:id="rId6"/>
     <sheet name="12Jan2024 152501" sheetId="8" r:id="rId7"/>
     <sheet name="17Jan2024 175835" sheetId="9" r:id="rId8"/>
+    <sheet name="06Feb2024 152311" r:id="rId12" sheetId="10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="667">
   <si>
     <t>Stock Name</t>
   </si>
@@ -1854,13 +1855,188 @@
   </si>
   <si>
     <t>22.25</t>
+  </si>
+  <si>
+    <t>Atok-Big Wedge Co., Inc.</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>4.70</t>
+  </si>
+  <si>
+    <t>7.40</t>
+  </si>
+  <si>
+    <t>4.40</t>
+  </si>
+  <si>
+    <t>4.93</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>APC Group, Inc.</t>
+  </si>
+  <si>
+    <t>APC</t>
+  </si>
+  <si>
+    <t>0.222</t>
+  </si>
+  <si>
+    <t>0.203</t>
+  </si>
+  <si>
+    <t>Asia United Bank Corporation</t>
+  </si>
+  <si>
+    <t>AUB</t>
+  </si>
+  <si>
+    <t>35.00</t>
+  </si>
+  <si>
+    <t>53.90</t>
+  </si>
+  <si>
+    <t>35.93</t>
+  </si>
+  <si>
+    <t>59.45</t>
+  </si>
+  <si>
+    <t>29.05</t>
+  </si>
+  <si>
+    <t>39.63</t>
+  </si>
+  <si>
+    <t>0.064</t>
+  </si>
+  <si>
+    <t>0.056</t>
+  </si>
+  <si>
+    <t>0.067</t>
+  </si>
+  <si>
+    <t>0.253</t>
+  </si>
+  <si>
+    <t>8.89</t>
+  </si>
+  <si>
+    <t>GMA Holdings, Inc.</t>
+  </si>
+  <si>
+    <t>GMAP</t>
+  </si>
+  <si>
+    <t>12.70</t>
+  </si>
+  <si>
+    <t>7.34</t>
+  </si>
+  <si>
+    <t>8.47</t>
+  </si>
+  <si>
+    <t>0.091</t>
+  </si>
+  <si>
+    <t>0.093</t>
+  </si>
+  <si>
+    <t>Petron Corporation</t>
+  </si>
+  <si>
+    <t>PCOR</t>
+  </si>
+  <si>
+    <t>2.50</t>
+  </si>
+  <si>
+    <t>3.13</t>
+  </si>
+  <si>
+    <t>Philippine Realty and Holdings Corporation</t>
+  </si>
+  <si>
+    <t>RLT</t>
+  </si>
+  <si>
+    <t>0.150</t>
+  </si>
+  <si>
+    <t>0.235</t>
+  </si>
+  <si>
+    <t>0.119</t>
+  </si>
+  <si>
+    <t>0.157</t>
+  </si>
+  <si>
+    <t>1.35</t>
+  </si>
+  <si>
+    <t>3.46</t>
+  </si>
+  <si>
+    <t>2.31</t>
+  </si>
+  <si>
+    <t>0.78</t>
+  </si>
+  <si>
+    <t>Victorias Milling Company, Inc.</t>
+  </si>
+  <si>
+    <t>VMC</t>
+  </si>
+  <si>
+    <t>3.80</t>
+  </si>
+  <si>
+    <t>2.10</t>
+  </si>
+  <si>
+    <t>2.53</t>
+  </si>
+  <si>
+    <t>2.64</t>
+  </si>
+  <si>
+    <t>1.76</t>
+  </si>
+  <si>
+    <t>22.30</t>
+  </si>
+  <si>
+    <t>34.00</t>
+  </si>
+  <si>
+    <t>22.67</t>
+  </si>
+  <si>
+    <t>0.083</t>
+  </si>
+  <si>
+    <t>0.066</t>
+  </si>
+  <si>
+    <t>0.087</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="57" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="64" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -2148,8 +2324,43 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2167,6 +2378,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="9ACD32"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2180,7 +2396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2239,6 +2455,13 @@
     <xf numFmtId="0" fontId="54" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="55" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="56" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="57" fillId="2" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="58" fillId="2" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="59" fillId="2" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="60" fillId="2" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="61" fillId="2" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="62" fillId="2" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="63" fillId="2" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2559,13 +2782,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="52.1796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="26.6328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -3444,6 +3667,580 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="41.69140625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.2890625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.03515625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="13.51953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="13.12109375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="19.0546875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="26.59375" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="58">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="59">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="60">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="61">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="62">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="63">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="64">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>609</v>
+      </c>
+      <c r="B2" t="s">
+        <v>610</v>
+      </c>
+      <c r="C2" t="s">
+        <v>611</v>
+      </c>
+      <c r="D2" t="s">
+        <v>612</v>
+      </c>
+      <c r="E2" t="s">
+        <v>613</v>
+      </c>
+      <c r="F2" t="s">
+        <v>614</v>
+      </c>
+      <c r="G2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>616</v>
+      </c>
+      <c r="B3" t="s">
+        <v>617</v>
+      </c>
+      <c r="C3" t="s">
+        <v>618</v>
+      </c>
+      <c r="D3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E3" t="s">
+        <v>619</v>
+      </c>
+      <c r="F3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G3" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>431</v>
+      </c>
+      <c r="B4" t="s">
+        <v>432</v>
+      </c>
+      <c r="C4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" t="s">
+        <v>433</v>
+      </c>
+      <c r="E4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F4" t="s">
+        <v>253</v>
+      </c>
+      <c r="G4" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>620</v>
+      </c>
+      <c r="B5" t="s">
+        <v>621</v>
+      </c>
+      <c r="C5" t="s">
+        <v>622</v>
+      </c>
+      <c r="D5" t="s">
+        <v>623</v>
+      </c>
+      <c r="E5" t="s">
+        <v>326</v>
+      </c>
+      <c r="F5" t="s">
+        <v>624</v>
+      </c>
+      <c r="G5" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>383</v>
+      </c>
+      <c r="D6" t="s">
+        <v>625</v>
+      </c>
+      <c r="E6" t="s">
+        <v>626</v>
+      </c>
+      <c r="F6" t="s">
+        <v>627</v>
+      </c>
+      <c r="G6" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>628</v>
+      </c>
+      <c r="D7" t="s">
+        <v>567</v>
+      </c>
+      <c r="E7" t="s">
+        <v>629</v>
+      </c>
+      <c r="F7" t="s">
+        <v>630</v>
+      </c>
+      <c r="G7" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>437</v>
+      </c>
+      <c r="B8" t="s">
+        <v>438</v>
+      </c>
+      <c r="C8" t="s">
+        <v>440</v>
+      </c>
+      <c r="D8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E8" t="s">
+        <v>440</v>
+      </c>
+      <c r="F8" t="s">
+        <v>631</v>
+      </c>
+      <c r="G8" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>442</v>
+      </c>
+      <c r="B9" t="s">
+        <v>443</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>444</v>
+      </c>
+      <c r="E9" t="s">
+        <v>445</v>
+      </c>
+      <c r="F9" t="s">
+        <v>446</v>
+      </c>
+      <c r="G9" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>307</v>
+      </c>
+      <c r="B10" t="s">
+        <v>308</v>
+      </c>
+      <c r="C10" t="s">
+        <v>362</v>
+      </c>
+      <c r="D10" t="s">
+        <v>361</v>
+      </c>
+      <c r="E10" t="s">
+        <v>362</v>
+      </c>
+      <c r="F10" t="s">
+        <v>362</v>
+      </c>
+      <c r="G10" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>452</v>
+      </c>
+      <c r="B11" t="s">
+        <v>453</v>
+      </c>
+      <c r="C11" t="s">
+        <v>632</v>
+      </c>
+      <c r="D11" t="s">
+        <v>455</v>
+      </c>
+      <c r="E11" t="s">
+        <v>456</v>
+      </c>
+      <c r="F11" t="s">
+        <v>457</v>
+      </c>
+      <c r="G11" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>633</v>
+      </c>
+      <c r="B12" t="s">
+        <v>634</v>
+      </c>
+      <c r="C12" t="s">
+        <v>558</v>
+      </c>
+      <c r="D12" t="s">
+        <v>635</v>
+      </c>
+      <c r="E12" t="s">
+        <v>636</v>
+      </c>
+      <c r="F12" t="s">
+        <v>637</v>
+      </c>
+      <c r="G12" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>469</v>
+      </c>
+      <c r="B13" t="s">
+        <v>470</v>
+      </c>
+      <c r="C13" t="s">
+        <v>638</v>
+      </c>
+      <c r="D13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" t="s">
+        <v>473</v>
+      </c>
+      <c r="F13" t="s">
+        <v>639</v>
+      </c>
+      <c r="G13" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>475</v>
+      </c>
+      <c r="B14" t="s">
+        <v>476</v>
+      </c>
+      <c r="C14" t="s">
+        <v>477</v>
+      </c>
+      <c r="D14" t="s">
+        <v>478</v>
+      </c>
+      <c r="E14" t="s">
+        <v>479</v>
+      </c>
+      <c r="F14" t="s">
+        <v>480</v>
+      </c>
+      <c r="G14" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>640</v>
+      </c>
+      <c r="B15" t="s">
+        <v>641</v>
+      </c>
+      <c r="C15" t="s">
+        <v>560</v>
+      </c>
+      <c r="D15" t="s">
+        <v>611</v>
+      </c>
+      <c r="E15" t="s">
+        <v>642</v>
+      </c>
+      <c r="F15" t="s">
+        <v>643</v>
+      </c>
+      <c r="G15" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>644</v>
+      </c>
+      <c r="B16" t="s">
+        <v>645</v>
+      </c>
+      <c r="C16" t="s">
+        <v>646</v>
+      </c>
+      <c r="D16" t="s">
+        <v>647</v>
+      </c>
+      <c r="E16" t="s">
+        <v>648</v>
+      </c>
+      <c r="F16" t="s">
+        <v>649</v>
+      </c>
+      <c r="G16" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>586</v>
+      </c>
+      <c r="B17" t="s">
+        <v>587</v>
+      </c>
+      <c r="C17" t="s">
+        <v>650</v>
+      </c>
+      <c r="D17" t="s">
+        <v>482</v>
+      </c>
+      <c r="E17" t="s">
+        <v>250</v>
+      </c>
+      <c r="F17" t="s">
+        <v>589</v>
+      </c>
+      <c r="G17" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>590</v>
+      </c>
+      <c r="B18" t="s">
+        <v>591</v>
+      </c>
+      <c r="C18" t="s">
+        <v>338</v>
+      </c>
+      <c r="D18" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" t="s">
+        <v>377</v>
+      </c>
+      <c r="F18" t="s">
+        <v>278</v>
+      </c>
+      <c r="G18" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>370</v>
+      </c>
+      <c r="B19" t="s">
+        <v>371</v>
+      </c>
+      <c r="C19" t="s">
+        <v>483</v>
+      </c>
+      <c r="D19" t="s">
+        <v>651</v>
+      </c>
+      <c r="E19" t="s">
+        <v>593</v>
+      </c>
+      <c r="F19" t="s">
+        <v>652</v>
+      </c>
+      <c r="G19" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>550</v>
+      </c>
+      <c r="B20" t="s">
+        <v>551</v>
+      </c>
+      <c r="C20" t="s">
+        <v>653</v>
+      </c>
+      <c r="D20" t="s">
+        <v>306</v>
+      </c>
+      <c r="E20" t="s">
+        <v>461</v>
+      </c>
+      <c r="F20" t="s">
+        <v>552</v>
+      </c>
+      <c r="G20" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>654</v>
+      </c>
+      <c r="B21" t="s">
+        <v>655</v>
+      </c>
+      <c r="C21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D21" t="s">
+        <v>656</v>
+      </c>
+      <c r="E21" t="s">
+        <v>657</v>
+      </c>
+      <c r="F21" t="s">
+        <v>658</v>
+      </c>
+      <c r="G21" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" t="s">
+        <v>276</v>
+      </c>
+      <c r="D22" t="s">
+        <v>659</v>
+      </c>
+      <c r="E22" t="s">
+        <v>606</v>
+      </c>
+      <c r="F22" t="s">
+        <v>660</v>
+      </c>
+      <c r="G22" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>492</v>
+      </c>
+      <c r="B23" t="s">
+        <v>493</v>
+      </c>
+      <c r="C23" t="s">
+        <v>661</v>
+      </c>
+      <c r="D23" t="s">
+        <v>662</v>
+      </c>
+      <c r="E23" t="s">
+        <v>495</v>
+      </c>
+      <c r="F23" t="s">
+        <v>663</v>
+      </c>
+      <c r="G23" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>229</v>
+      </c>
+      <c r="B24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C24" t="s">
+        <v>664</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" t="s">
+        <v>665</v>
+      </c>
+      <c r="F24" t="s">
+        <v>666</v>
+      </c>
+      <c r="G24" t="s">
+        <v>615</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -3455,13 +4252,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="52.1796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="26.6328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -4351,13 +5148,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="47.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="47.453125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="26.6328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -4994,13 +5791,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="45.36328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="26.6328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -5660,13 +6457,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="45.36328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="26.6328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -6188,13 +6985,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="52.1796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="26.6328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -6810,13 +7607,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="52.1796875" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.26953125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.0" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.54296875" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.08984375" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.08984375" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="26.6328125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -7478,13 +8275,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="52.1796875" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.26953125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.0" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.54296875" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.08984375" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.08984375" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="26.6328125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>